<commit_message>
revise progress check 2.2
</commit_message>
<xml_diff>
--- a/ch02-describing-data-tables-graphs/check-2.2.xlsx
+++ b/ch02-describing-data-tables-graphs/check-2.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\statistics-11-edition-exercises\ch02-describing-data-tables-graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936894A1-47A8-4D88-95B5-CDDD753CC494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCE5A31-2F3C-4B58-9E6F-2B91E7B75BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
   <si>
     <r>
       <t xml:space="preserve">Progress Check *2.2 </t>
@@ -270,15 +270,6 @@
     <t>Frequency Distribution Table</t>
   </si>
   <si>
-    <t>intervals</t>
-  </si>
-  <si>
-    <t>interval size</t>
-  </si>
-  <si>
-    <t>(max - min) / # interval</t>
-  </si>
-  <si>
     <t>start interval</t>
   </si>
   <si>
@@ -295,13 +286,82 @@
   </si>
   <si>
     <t>Frequency</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Data Analysis Tools</t>
+  </si>
+  <si>
+    <t>64.5–69.5</t>
+  </si>
+  <si>
+    <t>Model Answer</t>
+  </si>
+  <si>
+    <t>IQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> f</t>
+  </si>
+  <si>
+    <t>120–124</t>
+  </si>
+  <si>
+    <t>115–119</t>
+  </si>
+  <si>
+    <t>110–114</t>
+  </si>
+  <si>
+    <t>105–109</t>
+  </si>
+  <si>
+    <t>100–104</t>
+  </si>
+  <si>
+    <t>95–99</t>
+  </si>
+  <si>
+    <t>90–94</t>
+  </si>
+  <si>
+    <t>85–89</t>
+  </si>
+  <si>
+    <t>80–84</t>
+  </si>
+  <si>
+    <t>75–79</t>
+  </si>
+  <si>
+    <t>70–74</t>
+  </si>
+  <si>
+    <t>65–69</t>
+  </si>
+  <si>
+    <t>bins</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>(max - min) / # size</t>
+  </si>
+  <si>
+    <t>My Endeavor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,6 +401,14 @@
     <font>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -387,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -398,6 +466,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -1115,497 +1184,743 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A865D757-7DCB-4CC0-8674-FDE4004B69E3}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9:H15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:18">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B7" s="3">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B8" s="3">
         <v>71</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="N8" t="s">
+        <v>72</v>
+      </c>
+      <c r="O8">
+        <f>_xlfn.CEILING.MATH((B41-B7)/O9,5)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9">
+        <f>_xlfn.FLOOR.MATH(B41-B7,10)/G8</f>
+        <v>10</v>
+      </c>
+      <c r="H9" t="s">
+        <v>73</v>
+      </c>
+      <c r="N9" t="s">
+        <v>71</v>
+      </c>
+      <c r="O9">
+        <v>12</v>
+      </c>
+      <c r="P9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="16.5" thickBot="1">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>80</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
         <v>46</v>
       </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3">
-        <v>75</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G13" t="s">
         <v>47</v>
       </c>
-      <c r="G4">
-        <f>_xlfn.FLOOR.MATH(B36-B2,10)/G3</f>
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3">
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N13" t="s">
+        <v>57</v>
+      </c>
+      <c r="O13" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>57</v>
+      </c>
+      <c r="R13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>84</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" ref="E14:E19" si="0">F14&amp;"-"&amp;G14</f>
+        <v>69-78</v>
+      </c>
+      <c r="F14" s="3">
+        <f>B7</f>
+        <v>69</v>
+      </c>
+      <c r="G14" s="3">
+        <f>F14+G9-1</f>
+        <v>78</v>
+      </c>
+      <c r="H14">
+        <f t="array" ref="H14:H20">FREQUENCY(B7:B41,F14:F19)</f>
+        <v>1</v>
+      </c>
+      <c r="K14" s="4">
+        <v>69</v>
+      </c>
+      <c r="L14" s="5">
+        <v>1</v>
+      </c>
+      <c r="N14" t="s">
+        <v>59</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>65</v>
+      </c>
+      <c r="R14">
+        <f t="array" ref="R14:R26">FREQUENCY(B7:B41,Q14:Q26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3">
+        <v>85</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>79-88</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" ref="F15:F20" si="1">G14+1</f>
         <v>79</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3">
-        <v>80</v>
-      </c>
-      <c r="F8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3">
-        <v>84</v>
-      </c>
-      <c r="F9" s="3">
-        <f>B2</f>
-        <v>69</v>
-      </c>
-      <c r="G9" s="3">
-        <f>F9+G4-1</f>
-        <v>78</v>
-      </c>
-      <c r="H9">
-        <f t="array" ref="H9:H15">FREQUENCY(B2:B36,F9:F14)</f>
+      <c r="G15" s="3">
+        <f>F15+G9-1</f>
+        <v>88</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="K15" s="4">
+        <v>79</v>
+      </c>
+      <c r="L15" s="5">
+        <v>4</v>
+      </c>
+      <c r="N15" t="s">
+        <v>60</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>70</v>
+      </c>
+      <c r="R15">
         <v>1</v>
       </c>
-      <c r="I9" t="str">
-        <f>F9&amp;"-"&amp;G9</f>
-        <v>69-78</v>
-      </c>
-      <c r="K9" s="4">
-        <v>69</v>
-      </c>
-      <c r="L9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3">
-        <v>85</v>
-      </c>
-      <c r="F10" s="3">
-        <f>G9+1</f>
-        <v>79</v>
-      </c>
-      <c r="G10" s="3">
-        <f>F10+G4-1</f>
-        <v>88</v>
-      </c>
-      <c r="H10">
-        <v>4</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" ref="I10:I14" si="0">F10&amp;"-"&amp;G10</f>
-        <v>79-88</v>
-      </c>
-      <c r="K10" s="4">
-        <v>79</v>
-      </c>
-      <c r="L10" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" t="s">
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B16" s="3">
         <v>86</v>
       </c>
-      <c r="F11" s="3">
-        <f>G10+1</f>
-        <v>89</v>
-      </c>
-      <c r="G11" s="3">
-        <f>F11+G4-1</f>
-        <v>98</v>
-      </c>
-      <c r="H11">
-        <v>7</v>
-      </c>
-      <c r="I11" t="str">
+      <c r="E16" t="str">
         <f t="shared" si="0"/>
         <v>89-98</v>
       </c>
-      <c r="K11" s="4">
+      <c r="F16" s="3">
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
-      <c r="L11" s="5">
+      <c r="G16" s="3">
+        <f>F16+G9-1</f>
+        <v>98</v>
+      </c>
+      <c r="H16">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" t="s">
+      <c r="K16" s="4">
+        <v>89</v>
+      </c>
+      <c r="L16" s="5">
+        <v>7</v>
+      </c>
+      <c r="N16" t="s">
+        <v>61</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="Q16">
+        <v>75</v>
+      </c>
+      <c r="R16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B17" s="3">
         <v>87</v>
       </c>
-      <c r="F12" s="3">
-        <f>G11+1</f>
-        <v>99</v>
-      </c>
-      <c r="G12" s="3">
-        <f>F12+G4-1</f>
-        <v>108</v>
-      </c>
-      <c r="H12">
-        <v>13</v>
-      </c>
-      <c r="I12" t="str">
+      <c r="E17" t="str">
         <f t="shared" si="0"/>
         <v>99-108</v>
       </c>
-      <c r="K12" s="4">
+      <c r="F17" s="3">
+        <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="L12" s="5">
+      <c r="G17" s="3">
+        <f>F17+G9-1</f>
+        <v>108</v>
+      </c>
+      <c r="H17">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" t="s">
+      <c r="K17" s="4">
+        <v>99</v>
+      </c>
+      <c r="L17" s="5">
+        <v>13</v>
+      </c>
+      <c r="N17" t="s">
+        <v>62</v>
+      </c>
+      <c r="O17">
+        <v>3</v>
+      </c>
+      <c r="Q17">
+        <v>80</v>
+      </c>
+      <c r="R17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B18" s="3">
         <v>89</v>
       </c>
-      <c r="F13" s="3">
-        <f>G12+1</f>
-        <v>109</v>
-      </c>
-      <c r="G13" s="3">
-        <f>F13+G4-1</f>
-        <v>118</v>
-      </c>
-      <c r="H13">
-        <v>7</v>
-      </c>
-      <c r="I13" t="str">
+      <c r="E18" t="str">
         <f t="shared" si="0"/>
         <v>109-118</v>
       </c>
-      <c r="K13" s="4">
+      <c r="F18" s="3">
+        <f t="shared" si="1"/>
         <v>109</v>
       </c>
-      <c r="L13" s="5">
+      <c r="G18" s="3">
+        <f>F18+G9-1</f>
+        <v>118</v>
+      </c>
+      <c r="H18">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" t="s">
+      <c r="K18" s="4">
+        <v>109</v>
+      </c>
+      <c r="L18" s="5">
+        <v>7</v>
+      </c>
+      <c r="N18" t="s">
+        <v>63</v>
+      </c>
+      <c r="O18">
+        <v>4</v>
+      </c>
+      <c r="Q18">
+        <v>85</v>
+      </c>
+      <c r="R18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B19" s="3">
         <v>90</v>
       </c>
-      <c r="F14" s="3">
-        <f>G13+1</f>
-        <v>119</v>
-      </c>
-      <c r="G14" s="3">
-        <f>F14+G4-1</f>
-        <v>128</v>
-      </c>
-      <c r="H14">
-        <v>2</v>
-      </c>
-      <c r="I14" t="str">
+      <c r="E19" t="str">
         <f t="shared" si="0"/>
         <v>119-128</v>
       </c>
-      <c r="K14" s="4">
+      <c r="F19" s="3">
+        <f t="shared" si="1"/>
         <v>119</v>
       </c>
-      <c r="L14" s="5">
+      <c r="G19" s="3">
+        <f>F19+G9-1</f>
+        <v>128</v>
+      </c>
+      <c r="H19">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" t="s">
+      <c r="K19" s="4">
+        <v>119</v>
+      </c>
+      <c r="L19" s="5">
+        <v>2</v>
+      </c>
+      <c r="N19" t="s">
+        <v>64</v>
+      </c>
+      <c r="O19">
+        <v>6</v>
+      </c>
+      <c r="Q19">
+        <v>90</v>
+      </c>
+      <c r="R19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B20" s="3">
         <v>90</v>
       </c>
-      <c r="F15" s="3">
-        <f>G14+1</f>
+      <c r="F20" s="3">
+        <f t="shared" si="1"/>
         <v>129</v>
       </c>
-      <c r="H15">
+      <c r="H20">
         <v>1</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K20" s="4">
         <v>129</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L20" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A16" t="s">
+      <c r="N20" t="s">
+        <v>65</v>
+      </c>
+      <c r="O20">
+        <v>7</v>
+      </c>
+      <c r="Q20">
+        <v>95</v>
+      </c>
+      <c r="R20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B21" s="3">
         <v>90</v>
       </c>
-      <c r="K16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L16" s="6">
+      <c r="G21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21">
+        <f>SUM(H14:H20)</f>
+        <v>35</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" t="s">
+      <c r="N21" t="s">
+        <v>66</v>
+      </c>
+      <c r="O21">
+        <v>4</v>
+      </c>
+      <c r="Q21">
+        <v>100</v>
+      </c>
+      <c r="R21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B22" s="3">
         <v>90</v>
       </c>
-      <c r="L17">
-        <f>SUM(L9:L15)</f>
+      <c r="K22" t="s">
+        <v>52</v>
+      </c>
+      <c r="L22">
+        <f>SUM(L14:L20)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" t="s">
+      <c r="N22" t="s">
+        <v>67</v>
+      </c>
+      <c r="O22">
+        <v>3</v>
+      </c>
+      <c r="Q22">
+        <v>105</v>
+      </c>
+      <c r="R22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B23" s="3">
         <v>91</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" t="s">
+      <c r="N23" t="s">
+        <v>68</v>
+      </c>
+      <c r="O23">
+        <v>3</v>
+      </c>
+      <c r="Q23">
+        <v>110</v>
+      </c>
+      <c r="R23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B24" s="3">
         <v>93</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" t="s">
+      <c r="N24" t="s">
+        <v>69</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>115</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B25" s="3">
         <v>94</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" t="s">
+      <c r="N25" t="s">
+        <v>70</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>120</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B26" s="3">
         <v>95</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" t="s">
+      <c r="N26" t="s">
+        <v>52</v>
+      </c>
+      <c r="O26">
+        <f>SUM(O14:O25)</f>
+        <v>35</v>
+      </c>
+      <c r="Q26">
+        <v>125</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B27" s="3">
         <v>95</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" t="s">
+      <c r="Q27" t="s">
+        <v>52</v>
+      </c>
+      <c r="R27">
+        <f>SUM(R14:R26)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B28" s="3">
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
-      <c r="A24" t="s">
+    <row r="29" spans="1:18">
+      <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B29" s="3">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
-      <c r="A25" t="s">
+    <row r="30" spans="1:18">
+      <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B30" s="3">
         <v>98</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" t="s">
+      <c r="E30" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B31" s="3">
         <v>99</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" t="s">
+      <c r="E31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B32" s="3">
         <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="3">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="3">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="3">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="3">
-        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B33" s="3">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B34" s="3">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B35" s="3">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B41" s="3">
         <v>123</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K9:K15">
-    <sortCondition ref="K9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K14:K20">
+    <sortCondition ref="K14"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>